<commit_message>
-allows three digits following [q,w,e,r] special event shortcut when...
the corresponding slider max value is greater than 100.  Be aware that when this is true three digits must be entered so a leading zero is required for values less than 100.  
-changes Windows keyboard shortcut to remove background curve to CTRL+SHIFT+h
-corrects keyboardshortcuts help page
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -124,18 +124,6 @@
     <t>Desktop ScreenShot</t>
   </si>
   <si>
-    <t>q,w,e,r + &lt;i&gt;nn&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>Quick Custom Event</t>
-  </si>
-  <si>
-    <t>v + &lt;i&gt;nnn&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>Quick PID SV</t>
-  </si>
-  <si>
     <t>Full Screen Mode</t>
   </si>
   <si>
@@ -149,9 +137,6 @@
   </si>
   <si>
     <t>t\u00A0\u00A0\u00A0[Windows: CTRL+SHIFT+t]</t>
-  </si>
-  <si>
-    <t>h\u00A0\u00A0\u00A0[Windows: CTRL+SHIFT+h]</t>
   </si>
   <si>
     <t>f\u00A0\u00A0\u00A0[Windows:  CTRL+SHIFT+f]</t>
@@ -161,7 +146,22 @@
 When Keyboard Shortcuts are OFF adds a custom event</t>
   </si>
   <si>
-    <t>ALT+h\u00A0\u00A0\u00A0[Windows: CTRL+ALT+h]</t>
+    <t>ALT+h\u00A0\u00A0\u00A0[Windows: CTRL+SHIFT+h]</t>
+  </si>
+  <si>
+    <t>h\u00A0\u00A0\u00A0[Windows: CTRL+h]</t>
+  </si>
+  <si>
+    <t>q,w,e,r + &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>Quick PID SV Entry.  Value is a three digit number.  For values less than 100 must be entered with a leading zero, e.g. 'v075'.</t>
+  </si>
+  <si>
+    <t>v +  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Special Event Entry.  The keys q,w,e, and r correspond to special events 1,2,3 and 4.  A two digit numeric value must follow the shortcut letter, e.g. 'q75', when the correspoding event slider max value is 100 or less (default setting).   When the slider max value is greater than 100, three digits must be entered and for values less that 100 a leading zero is required, e.g. 'q075'.  </t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,12 +530,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -575,7 +575,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>24</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>25</v>
@@ -703,29 +703,30 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- refactoring for reduced startup time - reorganizes the macOS build setup to a more standardized structure - adds PDF as export format of roast, production and ranking reports - adds "PDF Report" as additional format to autosave
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -189,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -219,12 +219,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,7 +279,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,17 +356,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.21"/>
@@ -594,7 +588,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
- improved rendering of cursor coordinates - allow to deactivate cursor coordinates via key d - adds cursor coordinate clamp modes toggled by key z - have zoom follow respecting the cursor coordinates mode (temp vs RoR) - deactivate the MPL busy cursor on slow MPL processing like full redraws - updates lxml and MPL libs
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">KEYBOARD SHORTCUTS</t>
   </si>
@@ -71,7 +71,13 @@
     <t xml:space="preserve">d</t>
   </si>
   <si>
-    <t xml:space="preserve">Toggle xy scale (T/Delta)</t>
+    <t xml:space="preserve">Toggle xy cursor mode (off/temp/delta)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle xy cursor clamp mode (off/BT/ET/BTB/ETB)</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
@@ -360,15 +366,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.21"/>
   </cols>
   <sheetData>
@@ -441,7 +447,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -505,7 +511,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -517,15 +523,15 @@
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -583,6 +589,14 @@
       </c>
       <c r="B27" s="1" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds LCD cursor showing readings at cursor position while not recording
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">KEYBOARD SHORTCUTS</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle xy cursor clamp mode (off/BT/ET/BTB/ETB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle LCD cursor (off/profile/template)</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
@@ -366,13 +372,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.21"/>
@@ -455,7 +461,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -519,7 +525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -531,15 +537,15 @@
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -597,6 +603,14 @@
       </c>
       <c r="B28" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds shortcut to toggle Playback Events by hitting the j key; state visually indicated by background profile color - adds delta projection flag and save projection flag state in app settings - removes extra settings save from dialog exit for speed up - restrict setsv() on Fuji PXF PIDs to integers
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">KEYBOARD SHORTCUTS</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle PID mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle Playback Events</t>
   </si>
   <si>
     <t xml:space="preserve">h\u00A0\u00A0\u00A0[Windows: CTRL+h]</t>
@@ -378,13 +384,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.21"/>
@@ -531,7 +537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -547,7 +553,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -559,15 +565,15 @@
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -625,6 +631,14 @@
       </c>
       <c r="B30" s="1" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fix axis defaults button action - hardens manual temperature entry - hardens marking of input fields in RoastProperties - fixes entries in Release History - fixes overlap checking for off screen custom event annotations - changes the conditions for the automatic markDROP action on OFF, now bound to the autoDROP flag - fixes settings devices entries for devive=0 (PID)
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -83,7 +83,7 @@
     <t xml:space="preserve">u</t>
   </si>
   <si>
-    <t xml:space="preserve">Toggle LCD cursor (off/profile/template)</t>
+    <t xml:space="preserve">Toggle LCD cursor (off/profile/background)</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
@@ -387,10 +387,10 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.21"/>

</xml_diff>

<commit_message>
- removes support for Trobrat and Typhoon machines - removes Russian localization - adds Ukrainian localization
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -56,7 +56,35 @@
     <t xml:space="preserve">Autosave</t>
   </si>
   <si>
-    <t xml:space="preserve">CRTL+N</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMMAND-N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\u00A0\u00A0\u00A0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[Windows: CRTL+N]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Autosave + Reset + START</t>
@@ -140,7 +168,7 @@
     <t xml:space="preserve">Load background profile</t>
   </si>
   <si>
-    <t xml:space="preserve">ALT+h\u00A0\u00A0\u00A0[Windows: CTRL+SHIFT+h]</t>
+    <t xml:space="preserve">OPTION+h\u00A0\u00A0\u00A0[Windows: CTRL+SHIFT+h]</t>
   </si>
   <si>
     <t xml:space="preserve">Remove background profile</t>
@@ -170,7 +198,35 @@
     <t xml:space="preserve">Inc/dec PID lookahead</t>
   </si>
   <si>
-    <t xml:space="preserve">CRTL 0-9</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMMAND 0-9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\u00A0\u00A0\u00A0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[Windows: CRTL 0-9]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Changes Event Button Palettes</t>
@@ -213,7 +269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,6 +298,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -386,11 +448,11 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.21"/>
@@ -441,7 +503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -593,7 +655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
- auto axis graph mode 1 and 2 do not alter show full setup - auto axis respects cooling phase only if COOL button is visible - new shortcut: COMMAND/CTRL +/-  to inc/dec graph resolution
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="184">
   <si>
     <t xml:space="preserve">KEYBOARD SHORTCUTS</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t xml:space="preserve">Inc/dec PID lookahead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⌘ +,- [Mac]\nCRTL +,- [Win]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inc/dec graph resolution</t>
   </si>
   <si>
     <t xml:space="preserve">⌘ 0-9 [Mac]\nCRTL 0-9 [Win]</t>
@@ -578,7 +584,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -600,6 +606,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -654,7 +666,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -671,15 +683,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -701,15 +717,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.15"/>
   </cols>
   <sheetData>
@@ -918,8 +934,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -964,6 +980,14 @@
       </c>
       <c r="B32" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -988,393 +1012,393 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="72.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="45.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="4" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="72.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="45.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="5" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>62</v>
+      <c r="A1" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>73</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>75</v>
+      <c r="A5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>77</v>
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>82</v>
+      <c r="A8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>84</v>
+      <c r="A9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>86</v>
+      <c r="A10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>88</v>
+      <c r="A11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>90</v>
+      <c r="A12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="C13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>97</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>99</v>
+      <c r="C15" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="A16" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="B16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>104</v>
+      <c r="D17" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>106</v>
+      <c r="A18" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>109</v>
       </c>
+      <c r="B19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>111</v>
+      <c r="A20" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>113</v>
+      <c r="A21" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="6" t="s">
         <v>116</v>
       </c>
+      <c r="B22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="6" t="s">
         <v>119</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="C26" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="C27" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>123</v>
+      <c r="A28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>133</v>
+      <c r="A29" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>135</v>
+      <c r="A30" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="A31" s="6" t="s">
         <v>138</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1423,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.58"/>
@@ -1407,7 +1431,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,219 +1439,219 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>142</v>
+      <c r="A3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>144</v>
+      <c r="C4" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>145</v>
+      <c r="A5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="6" t="s">
         <v>148</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>149</v>
       </c>
+      <c r="C7" s="7" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>151</v>
+      <c r="A8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="6" t="s">
         <v>154</v>
       </c>
+      <c r="B9" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>156</v>
+      <c r="C10" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>158</v>
+      <c r="A11" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="B12" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>163</v>
+      <c r="C13" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>165</v>
+      <c r="A14" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>167</v>
+      <c r="A15" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>169</v>
+      <c r="A16" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="6" t="s">
         <v>172</v>
       </c>
+      <c r="B17" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>174</v>
+      <c r="C18" s="7" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>176</v>
+      <c r="A19" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>178</v>
+      <c r="C20" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="6" t="s">
         <v>181</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixes some PT_BR translations of the MODBUS tab - fixes MODBUS scan - adds OPTION+B [Mac] / CTRL-SHIFT+B [Win] keyboard shortcut followed by two digits to fire corresponding custom event button action
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="186">
   <si>
     <t xml:space="preserve">KEYBOARD SHORTCUTS</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t xml:space="preserve">Quick PID SV Entry.  Value is a three digit number.  For values less than 100 must be entered with a leading zero, e.g. 'v075'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION+B + &lt;value&gt; [Mac]\nCTRL+SHIFT+B + &lt;value&gt; [Win]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire custom event button action. Value is a two digit number indicating the button number.</t>
   </si>
   <si>
     <t xml:space="preserve">F\nCTRL+SHIFT+F [Win]</t>
@@ -709,11 +715,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.11"/>
@@ -972,7 +978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -980,7 +986,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1016,393 +1029,393 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="31.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="72.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="72.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="45.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="4" width="9.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="4" width="9.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="C15" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1440,7 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
@@ -1436,7 +1449,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,219 +1457,219 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>155</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="C13" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="C20" s="6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- skip settings save on Shift-Alt
- skip creating settings cache and ask user to apply existing settings or settings from profile
- update keyboard shortcuts help
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\GitHub\artisan\doc\help_dialogs\Input_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004AA876-B8EC-4744-A652-B14B607A4132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keyboard Shortcuts" sheetId="1" r:id="rId1"/>
     <sheet name="Addl Shortcuts" sheetId="2" r:id="rId2"/>
     <sheet name="Menu Shortcuts" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="219">
   <si>
     <t>KEYBOARD SHORTCUTS</t>
   </si>
@@ -51,10 +57,6 @@
   </si>
   <si>
     <t>SPACE</t>
-  </si>
-  <si>
-    <t>When Keyboard Shortcuts are ON chooses the current button
-When Keyboard Shortcuts are OFF adds a custom event</t>
   </si>
   <si>
     <t>LEFT,RIGHT</t>
@@ -660,12 +662,38 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>When Keyboard Shortcuts are ON chooses the current button
+When Keyboard Shortcuts are OFF adds a custom event
+When Meter=NONE opens dialog to manually enter temperatures during roast</t>
+  </si>
+  <si>
+    <t>When starting Artisan</t>
+  </si>
+  <si>
+    <t>Skip Settings Load</t>
+  </si>
+  <si>
+    <t>Hold Shift+Option [Mac]\nHold Shift+Alt [Win]</t>
+  </si>
+  <si>
+    <t>When quiting Artisan</t>
+  </si>
+  <si>
+    <t>Skip Settings Save</t>
+  </si>
+  <si>
+    <t>When opening a profile (.alog file)</t>
+  </si>
+  <si>
+    <t>Skip creating settings cache and ask user to apply existing settings or settings from profile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -724,7 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -732,11 +760,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -753,7 +778,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -761,14 +786,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -806,7 +834,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -878,7 +906,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1051,11 +1079,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,260 +1129,260 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>51</v>
+        <v>210</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1364,484 +1392,517 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMJ40"/>
   <sheetViews>
-    <sheetView topLeftCell="C21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="72" style="5" customWidth="1"/>
-    <col min="4" max="4" width="74.7109375" style="5" customWidth="1"/>
-    <col min="5" max="1024" width="9.140625" style="5"/>
+    <col min="1" max="1" width="53" style="4" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="72" style="4" customWidth="1"/>
+    <col min="4" max="4" width="74.7109375" style="4" customWidth="1"/>
+    <col min="5" max="1024" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="B13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="5" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="8" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="B20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="B21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="B22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="8" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="5" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="B24" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="B25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="5" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="B26" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="5" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="B27" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="6" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="B28" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="5" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="B29" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="5" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="B30" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="5" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="B31" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="B32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="B33" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="B35" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="5" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="B36" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>167</v>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1851,7 +1912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
@@ -1867,7 +1928,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1875,219 +1936,219 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="10" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="10" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="10" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="10" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="10" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="10" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" s="10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="B11" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="10" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="B13" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C13" s="10" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C14" s="10" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="10" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="10" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="10" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="B18" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C18" s="10" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C19" s="10" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C20" s="10" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-downgrade pydantic for legacy windows
-update keyboard shortcuts help
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\GitHub\artisan\doc\help_dialogs\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D4C4F1-29EB-4FF6-9632-7346689B02BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C74CA40-ABBC-4DF4-A924-0D5B2E6EC19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="222">
   <si>
     <t>KEYBOARD SHORTCUTS</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>Detach IO Phidgets</t>
-  </si>
-  <si>
-    <t>⌘ click 'Control' Button [Mac]\nCTRL click 'Control' Button [Win]</t>
   </si>
   <si>
     <t>Toggle PID Standby on and off</t>
@@ -688,6 +685,18 @@
   </si>
   <si>
     <t>When quitting Artisan</t>
+  </si>
+  <si>
+    <t>⌘ click 'CONTROL' Button [Mac]\nCTRL click 'CONTROL' Button [Win]</t>
+  </si>
+  <si>
+    <t>⌘+PLUS, ⌘+MINUS [Mac]\nCTRL+SHIFT+PLUS, CTRL+MINUS [Win]</t>
+  </si>
+  <si>
+    <t>Increase or Decrease Graph Resolution %</t>
+  </si>
+  <si>
+    <t>Same as Config&gt;&gt; Curves&gt; UI tab&gt;&gt; Graph % +/-</t>
   </si>
 </sst>
 </file>
@@ -1086,18 +1095,18 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1105,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1129,15 +1138,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1145,7 +1154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1177,7 +1186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1194,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1217,7 +1226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1233,7 +1242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1241,7 +1250,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
@@ -1273,7 +1282,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1289,7 +1298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
@@ -1297,15 +1306,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -1369,7 +1378,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
@@ -1393,27 +1402,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ40"/>
+  <dimension ref="A1:AMJ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="53" style="4" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" style="4" customWidth="1"/>
     <col min="3" max="3" width="72" style="4" customWidth="1"/>
-    <col min="4" max="4" width="74.7109375" style="4" customWidth="1"/>
-    <col min="5" max="1024" width="9.140625" style="4"/>
+    <col min="4" max="4" width="74.7265625" style="4" customWidth="1"/>
+    <col min="5" max="1024" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
@@ -1427,7 +1436,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>76</v>
       </c>
@@ -1441,7 +1450,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>80</v>
       </c>
@@ -1455,7 +1464,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>84</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>86</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>88</v>
       </c>
@@ -1491,7 +1500,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>91</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>93</v>
       </c>
@@ -1513,7 +1522,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>95</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>97</v>
       </c>
@@ -1535,7 +1544,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>99</v>
       </c>
@@ -1546,7 +1555,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>101</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>104</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>106</v>
       </c>
@@ -1585,324 +1594,338 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="4" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="7" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="D21" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="D22" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="4" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="4" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="B26" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="4" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="4" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B28" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="5" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="B29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="4" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="B30" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" s="4" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="B31" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D30" s="4" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="B32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="D32" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="B33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="D33" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D34" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C35" s="4" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C36" s="4" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C38" s="4" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1919,236 +1942,236 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.26953125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="9" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="9" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7" s="9" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" s="9" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C9" s="9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C10" s="9" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" s="9" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="9" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C13" s="9" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="9" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C15" s="9" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C16" s="9" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="9" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C18" s="9" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="9" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C20" s="9" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- right-click EVENT input dialog remembers event type - a picked custom event can be removed using the backspace key - adds quick keyboard focused event slider input using numeric keys followed by the ENTER/RETURN key. The last digit can be removed by using the backspace key. - the quick custom event entry using the q, w, e and e key followed by number keys now requires the ENTER/RETURN key to establish the new value.  The last entered digit can be removed by using the backspace key. - adds keyboard shortcut annotations to View menu entries (buttons, sliders, control, and readings)
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Keyboard Shortcuts" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Addl Shortcuts" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Menu Shortcuts" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Keyboard Shortcuts" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Addl Shortcuts" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Menu Shortcuts" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -224,13 +224,13 @@
     <t xml:space="preserve">Q,W,E,R + &lt;value&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Quick Special Event Entry.  The keys q,w,e, and r correspond to special events 1,2,3 and 4.  A two digit numeric value must follow the shortcut letter, e.g. 'q75', when the corresponding event slider max value is 100 or less (default setting).   When the slider max value is greater than 100, three digits must be entered and for values less than 100 a leading zero is required, e.g. 'q075'.  </t>
+    <t xml:space="preserve">Quick Special Event Entry.  The keys q,w,e, and r correspond to special events 1,2,3 and 4. The new &lt;value&gt; is established using the ENTER/RETURN key. The last digit can be removed by using the backspace key.</t>
   </si>
   <si>
     <t xml:space="preserve">V +  &lt;value&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Quick PID SV Entry.  Value is a three digit number.  For values less than 100 must be entered with a leading zero, e.g. 'v075'.</t>
+    <t xml:space="preserve">Quick PID SV Entry. The new &lt;value&gt; is established using the ENTER/RETURN key. The last digit can be removed by using the backspace key.</t>
   </si>
   <si>
     <t xml:space="preserve">OPTION+B + &lt;value&gt; [Mac]\nCTRL+SHIFT+B + &lt;value&gt; [Win]</t>
@@ -792,44 +792,48 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -846,15 +850,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,7 +1010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1268,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1168,13 +1278,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1420,7 +1530,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>120</v>
       </c>
@@ -1434,7 +1544,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>124</v>
       </c>
@@ -1448,7 +1558,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>126</v>
       </c>
@@ -1462,7 +1572,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>128</v>
       </c>
@@ -1700,7 +1810,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1710,7 +1820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1722,13 +1832,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="35.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="8" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1744,217 +1854,217 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>153</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>155</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>186</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>162</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>192</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>195</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>197</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>199</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>202</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>204</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>206</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>208</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>210</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>213</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>140</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>217</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>221</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>